<commit_message>
Changes performed on 10-20-2022
</commit_message>
<xml_diff>
--- a/dados_full_brasil.xlsx
+++ b/dados_full_brasil.xlsx
@@ -3090,7 +3090,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3174,7 +3174,7 @@
   <dimension ref="A1:Q967"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A913" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F939" activeCellId="0" sqref="F939"/>
+      <selection pane="topLeft" activeCell="L939" activeCellId="0" sqref="L939"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>